<commit_message>
installed capacity  graph added
</commit_message>
<xml_diff>
--- a/Calliope_Kenya/Models/4Nodes_No-Coffee/Graph_inputs.xlsx
+++ b/Calliope_Kenya/Models/4Nodes_No-Coffee/Graph_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\Calliope_Kenya\Models\4Nodes_No-Coffee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905A1B78-57DF-4005-A558-B84EA10880E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41345C3F-40CB-4FB9-BA79-D33034A63C66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9FB00E9D-CEB3-42BA-85F0-61134DCC4F6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{9FB00E9D-CEB3-42BA-85F0-61134DCC4F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Consumption Techs" sheetId="1" r:id="rId1"/>
@@ -673,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C088BFEB-5357-40AB-A001-86E2ED77B251}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF150A4-DE49-47F1-B3B1-E0F51365CAAD}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1091,7 @@
         <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
         <v>64</v>
@@ -1102,7 +1102,7 @@
         <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
xticks and unit issues are solved
</commit_message>
<xml_diff>
--- a/Calliope_Kenya/Models/4Nodes_No-Coffee/Graph_inputs.xlsx
+++ b/Calliope_Kenya/Models/4Nodes_No-Coffee/Graph_inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevo\Repositories\CIVICS_Kenya\Calliope_Kenya\Models\4Nodes_No-Coffee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\Calliope_Kenya\Models\4Nodes_No-Coffee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C60526-E233-41ED-806F-200B6DC145AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8129B5E9-11B0-4EE7-8AD7-5F17D01C1572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="6" xr2:uid="{9FB00E9D-CEB3-42BA-85F0-61134DCC4F6B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{9FB00E9D-CEB3-42BA-85F0-61134DCC4F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Consumption Techs" sheetId="1" r:id="rId1"/>
@@ -320,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -336,7 +336,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -638,12 +638,12 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -652,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -677,9 +677,9 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
@@ -687,7 +687,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -741,16 +741,16 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -761,7 +761,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -783,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -848,17 +848,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF150A4-DE49-47F1-B3B1-E0F51365CAAD}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
@@ -866,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -877,7 +877,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -888,7 +888,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -899,7 +899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -910,7 +910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -921,7 +921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -932,7 +932,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -943,7 +943,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -954,7 +954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -965,7 +965,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -976,7 +976,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -987,7 +987,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -998,7 +998,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
@@ -1086,18 +1086,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>65</v>
       </c>
@@ -1121,13 +1121,13 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>64</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1192,14 +1192,14 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1224,21 +1224,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79EFBBC-D91E-4893-86C8-C299F0E0C218}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>

</xml_diff>